<commit_message>
Refactored Stored Proc code
</commit_message>
<xml_diff>
--- a/BballMVC/_Documentation/BballMVC_Doc.xlsx
+++ b/BballMVC/_Documentation/BballMVC_Doc.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\wwwroot\Test\mrroot123\mrroot123\BballMVCproject\BballMVC\_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A66F40A-6A4D-4F95-A7B2-CE44F8F024F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876A3BA0-08D4-4E05-AA2C-F210C434B779}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="3210" windowWidth="21600" windowHeight="12750" xr2:uid="{03DA9A79-FE21-4B9D-9E56-4EA80CA75797}"/>
+    <workbookView xWindow="4110" yWindow="1995" windowWidth="21600" windowHeight="12750" xr2:uid="{03DA9A79-FE21-4B9D-9E56-4EA80CA75797}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tables" sheetId="1" r:id="rId1"/>
-    <sheet name="References" sheetId="2" r:id="rId2"/>
+    <sheet name="Tasks" sheetId="3" r:id="rId1"/>
+    <sheet name="Tables" sheetId="1" r:id="rId2"/>
+    <sheet name="References" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
   <si>
     <t>Table</t>
   </si>
@@ -143,6 +144,12 @@
   </si>
   <si>
     <t>Bball.VbClasseslnterfaces</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
@@ -244,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -258,6 +265,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,10 +579,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80042610-4475-439E-8D8A-B99F3A7253D1}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DDC7D53-38AE-4E14-9D16-5C0AB081DB88}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -635,7 +669,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE5D99A2-B987-4E19-A171-ABA2F3A75912}">
   <dimension ref="A1:L13"/>
   <sheetViews>

</xml_diff>

<commit_message>
Changes since last push
</commit_message>
<xml_diff>
--- a/BballMVC/_Documentation/BballMVC_Doc.xlsx
+++ b/BballMVC/_Documentation/BballMVC_Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\wwwroot\Test\mrroot123\mrroot123\BballMVCproject\BballMVC\_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876A3BA0-08D4-4E05-AA2C-F210C434B779}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F06A15-C427-4DBC-AE2C-6220000D4BAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="1995" windowWidth="21600" windowHeight="12750" xr2:uid="{03DA9A79-FE21-4B9D-9E56-4EA80CA75797}"/>
+    <workbookView xWindow="1380" yWindow="465" windowWidth="24840" windowHeight="14820" activeTab="1" xr2:uid="{03DA9A79-FE21-4B9D-9E56-4EA80CA75797}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
   <si>
     <t>Table</t>
   </si>
@@ -150,6 +150,72 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Adjustments</t>
+  </si>
+  <si>
+    <t>AdjustmentsCodes</t>
+  </si>
+  <si>
+    <t>AdjustmentsDaily</t>
+  </si>
+  <si>
+    <t>BoxScoresLastSMin</t>
+  </si>
+  <si>
+    <t>Leaguelnfo</t>
+  </si>
+  <si>
+    <t>Lines</t>
+  </si>
+  <si>
+    <t>MatchupsResults</t>
+  </si>
+  <si>
+    <t>ParmTable</t>
+  </si>
+  <si>
+    <t>Plays</t>
+  </si>
+  <si>
+    <t>Seasonlnfo</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>TeamStats</t>
+  </si>
+  <si>
+    <t>TeamStatsAverages</t>
+  </si>
+  <si>
+    <t>TeamStrength</t>
+  </si>
+  <si>
+    <t>TodaysMatchups</t>
+  </si>
+  <si>
+    <t>TodaysPlays</t>
+  </si>
+  <si>
+    <t>UserLeagueParms</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>1 per BoxScore</t>
+  </si>
+  <si>
+    <t>1 per League</t>
+  </si>
+  <si>
+    <t>Multiple per Matchup</t>
+  </si>
+  <si>
+    <t>1 per SubSeason per Season per League</t>
   </si>
 </sst>
 </file>
@@ -582,7 +648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80042610-4475-439E-8D8A-B99F3A7253D1}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -606,17 +672,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DDC7D53-38AE-4E14-9D16-5C0AB081DB88}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" customWidth="1"/>
     <col min="2" max="2" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -661,6 +728,108 @@
       </c>
       <c r="C4" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -673,8 +842,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE5D99A2-B987-4E19-A171-ABA2F3A75912}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated TodaysMatchup for updated Table layout
</commit_message>
<xml_diff>
--- a/BballMVC/_Documentation/BballMVC_Doc.xlsx
+++ b/BballMVC/_Documentation/BballMVC_Doc.xlsx
@@ -8,20 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\wwwroot\Test\mrroot123\mrroot123\BballMVCproject\BballMVC\_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6478C151-BE69-439D-9F84-AB1618E93FC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C7D841-03C3-4D29-B095-08A41E8FE55F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26895" windowHeight="14505" activeTab="5" xr2:uid="{03DA9A79-FE21-4B9D-9E56-4EA80CA75797}"/>
+    <workbookView xWindow="1575" yWindow="405" windowWidth="26835" windowHeight="14535" activeTab="2" xr2:uid="{03DA9A79-FE21-4B9D-9E56-4EA80CA75797}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="3" r:id="rId1"/>
     <sheet name="Tables" sheetId="1" r:id="rId2"/>
     <sheet name="References" sheetId="2" r:id="rId3"/>
-    <sheet name="Adj Page" sheetId="4" r:id="rId4"/>
-    <sheet name="Adj Point Pct" sheetId="5" r:id="rId5"/>
-    <sheet name="BoxScore Seed Screen" sheetId="6" r:id="rId6"/>
+    <sheet name="DLLs" sheetId="7" r:id="rId4"/>
+    <sheet name="Adj Page" sheetId="4" r:id="rId5"/>
+    <sheet name="Adj Point Pct" sheetId="5" r:id="rId6"/>
+    <sheet name="BoxScore Seed Screen" sheetId="6" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tables!$A$1:$F$24</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,8 +39,57 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Keith</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{E9F86DB3-32F0-4C4D-B010-4B9243F98F96}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Table_Counts.sql</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Keith</author>
+  </authors>
+  <commentList>
+    <comment ref="B25" authorId="0" shapeId="0" xr:uid="{DB85BA36-67CC-42E5-A1D1-F06EF8F0A936}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">net45, 46 &amp; 47 all seem to have the same Unity.Mvc.dll
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="221">
   <si>
     <t>Table</t>
   </si>
@@ -388,13 +440,557 @@
   </si>
   <si>
     <t xml:space="preserve">  order by StartDate desc</t>
+  </si>
+  <si>
+    <t>UnityConfig.cs</t>
+  </si>
+  <si>
+    <t>using Unity;</t>
+  </si>
+  <si>
+    <t>5.11.1.0</t>
+  </si>
+  <si>
+    <t>Unity.Mvc</t>
+  </si>
+  <si>
+    <t>1.4.0.0</t>
+  </si>
+  <si>
+    <t>Unity.Mvc5</t>
+  </si>
+  <si>
+    <r>
+      <t>D:\My Documents\wwwroot\Test\MVCUsingUnity\packages\Unity.Mvc5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.1.4.0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\lib\</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>net45</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\Unity.Mvc5.dll</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>D:\My Documents\wwwroot\Test\mrroot123\mrroot123\BballMVCproject\packages\Unity.Mvc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.5.11.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\lib\</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>net47</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\Unity.Mvc.dll</t>
+    </r>
+  </si>
+  <si>
+    <t>Unity.Container</t>
+  </si>
+  <si>
+    <t>D:\My Documents\wwwroot\Test\mrroot123\mrroot123\BballMVCproject\packages\Unity.Container.5.11.6\lib\net47\Unity.Container.dll</t>
+  </si>
+  <si>
+    <t>5.11.6.0</t>
+  </si>
+  <si>
+    <r>
+      <t>D:\My Documents\wwwroot\Test\mrroot123\mrroot123\BballMVCproject\packages\Unity.Container</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.5.11.6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\lib\</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>net47</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\Unity.Container.dll</t>
+    </r>
+  </si>
+  <si>
+    <t>Unity.Abstractions</t>
+  </si>
+  <si>
+    <t>5.11.5.0</t>
+  </si>
+  <si>
+    <r>
+      <t>D:\My Documents\wwwroot\Test\mrroot123\mrroot123\BballMVCproject\packages\Unity.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5.11.5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\lib\</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>net47</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\Unity.Abstractions.dll</t>
+    </r>
+  </si>
+  <si>
+    <t>BBallMVC</t>
+  </si>
+  <si>
+    <t>System.Web.Mvc</t>
+  </si>
+  <si>
+    <t>5.2.3.0</t>
+  </si>
+  <si>
+    <r>
+      <t>D:\My Documents\wwwroot\Test\mrroot123\mrroot123\BballMVCproject\packages\Microsoft.AspNet.Mvc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.5.2.3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\lib</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\net45</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\System.Web.Mvc.dll</t>
+    </r>
+  </si>
+  <si>
+    <t>D:\My Documents\wwwroot\Test\mrroot123\mrroot123\BballMVCproject\packages\Unity.Abstractions.5.11.5\lib\net47\Unity.Abstractions.dll</t>
+  </si>
+  <si>
+    <t>Bball.Unity</t>
+  </si>
+  <si>
+    <t>D:\My Documents\wwwroot\Test\mrroot123\mrroot123\BballMVCproject\</t>
+  </si>
+  <si>
+    <t>\Unity.Mvc.5.11.1\lib\net47\Unity.Mvc.dll</t>
+  </si>
+  <si>
+    <t>D:\My Documents\wwwroot\Test\MVCUsingUnity\</t>
+  </si>
+  <si>
+    <t>\Unity.Mvc5.1.4.0\lib\net45\Unity.Mvc5.dll</t>
+  </si>
+  <si>
+    <t>\Microsoft.AspNet.Mvc.5.2.3\lib\net45\System.Web.Mvc.dll</t>
+  </si>
+  <si>
+    <t>\Unity.5.11.5\lib\net47\Unity.Abstractions.dll</t>
+  </si>
+  <si>
+    <t>\Unity.Container.5.11.6\lib\net47\Unity.Container.dll</t>
+  </si>
+  <si>
+    <t>\Unity.Abstractions.5.11.5\lib\net47\Unity.Abstractions.dll</t>
+  </si>
+  <si>
+    <t>packages</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>dll same</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Net Ver</t>
+  </si>
+  <si>
+    <t>Created</t>
+  </si>
+  <si>
+    <t>uspCalcTM - step 3</t>
+  </si>
+  <si>
+    <t>uspCalcTM - step 4</t>
+  </si>
+  <si>
+    <t>Manually</t>
+  </si>
+  <si>
+    <t>Adj Entry Modal</t>
+  </si>
+  <si>
+    <t>BAL.LoadBoxScores</t>
+  </si>
+  <si>
+    <t>Adjustment type descriptions</t>
+  </si>
+  <si>
+    <t>1 per type - around 7</t>
+  </si>
+  <si>
+    <t>Team, Injury, League, Misc</t>
+  </si>
+  <si>
+    <t>Stats for last 5 mins of 4th qtr</t>
+  </si>
+  <si>
+    <t>During Rotation update</t>
+  </si>
+  <si>
+    <t>TO BE implemented</t>
+  </si>
+  <si>
+    <t>Yesterday's results</t>
+  </si>
+  <si>
+    <t>As needed</t>
+  </si>
+  <si>
+    <t>Misc Parm info</t>
+  </si>
+  <si>
+    <t>If Team changes name, new entry created</t>
+  </si>
+  <si>
+    <t>1 per Active Team per league</t>
+  </si>
+  <si>
+    <t>empty - looks like TeamStatsAverages predesessor</t>
+  </si>
+  <si>
+    <t>probably not used</t>
+  </si>
+  <si>
+    <t>TM UI</t>
+  </si>
+  <si>
+    <t>1 per User</t>
+  </si>
+  <si>
+    <t>Name &amp; PW</t>
+  </si>
+  <si>
+    <t>1 per User per League</t>
+  </si>
+  <si>
+    <t>Gen calc info - GB, Wt, Pct</t>
+  </si>
+  <si>
+    <t>Old - use TodaysPlays</t>
+  </si>
+  <si>
+    <t>Recipients</t>
+  </si>
+  <si>
+    <t>AdjustmentsOtSide</t>
+  </si>
+  <si>
+    <t>Not created</t>
+  </si>
+  <si>
+    <t>1 per half side point per league - max 15 pts</t>
+  </si>
+  <si>
+    <t>Amt to adj OT depending on SideLine</t>
+  </si>
+  <si>
+    <t>1 per Recipient</t>
+  </si>
+  <si>
+    <t>Email of followers - make generic</t>
+  </si>
+  <si>
+    <t>1 per Game per Day per League per User</t>
+  </si>
+  <si>
+    <t>Deprecated</t>
+  </si>
+  <si>
+    <t>1 per Team per Day per GB per League per User</t>
+  </si>
+  <si>
+    <t>Team Avg 1, 2, 3PTers for GameBack</t>
+  </si>
+  <si>
+    <t>1 per Team per Day per GB per League</t>
+  </si>
+  <si>
+    <t>TS, Scored/Allowed &amp; BxSc &amp; TM Pcts</t>
+  </si>
+  <si>
+    <t>TMs used by TM UI</t>
+  </si>
+  <si>
+    <t>Sub Season St/End, Includes / Bypasses</t>
+  </si>
+  <si>
+    <t>TMs, Per, Mins, OT, Multi Yr</t>
+  </si>
+  <si>
+    <t>1 per Team per Game</t>
+  </si>
+  <si>
+    <t>Sum of Teams Adj for that day</t>
+  </si>
+  <si>
+    <t>DAL.AdjustmentsDailyDO</t>
+  </si>
+  <si>
+    <t>Max Date</t>
+  </si>
+  <si>
+    <t>Tomorrow</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>Yesterday</t>
+  </si>
+  <si>
+    <t>Today</t>
+  </si>
+  <si>
+    <t>GameDate</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>uspCalcTM - step 2 - uspInsertMatchupResults</t>
+  </si>
+  <si>
+    <t>uspCalcTM - step 2 - uspQueryCalcTeamStrength</t>
+  </si>
+  <si>
+    <t>Deprecated???</t>
+  </si>
+  <si>
+    <t>BU St Procs</t>
+  </si>
+  <si>
+    <t>What is @TmStrAdjPct</t>
+  </si>
+  <si>
+    <t>Doc all Tm Str</t>
+  </si>
+  <si>
+    <t>in CalcTMs - Part 4 Query tm</t>
+  </si>
+  <si>
+    <t>Unity Packages</t>
+  </si>
+  <si>
+    <t>5.11.7</t>
+  </si>
+  <si>
+    <t>Unity</t>
+  </si>
+  <si>
+    <t>5.11.6</t>
+  </si>
+  <si>
+    <t>5.11.8</t>
+  </si>
+  <si>
+    <t>5.11.1</t>
+  </si>
+  <si>
+    <t>5.11.5</t>
+  </si>
+  <si>
+    <t>Installed</t>
+  </si>
+  <si>
+    <t>Latest</t>
+  </si>
+  <si>
+    <t>MVC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Projects</t>
+  </si>
+  <si>
+    <r>
+      <t>D:\My Documents\wwwroot\Test\</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mrroot123</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\mrroot123\BballMVCproject\</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -422,6 +1018,34 @@
       <color rgb="FF222222"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -495,7 +1119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -535,6 +1159,18 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,6 +1189,99 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2810267</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>162699</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64B5F274-7CD6-4EA5-9841-DB6E3A81EE03}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="190500"/>
+          <a:ext cx="2810267" cy="5544324"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2686425</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>124667</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F688DBF4-48CA-4884-84D3-96F297FB27CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4333875" y="409575"/>
+          <a:ext cx="2686425" cy="6001592"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -601,7 +1330,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -947,10 +1676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80042610-4475-439E-8D8A-B99F3A7253D1}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C12" sqref="C12:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,12 +1687,33 @@
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="26">
+        <v>43989</v>
+      </c>
+      <c r="B2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -972,22 +1722,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DDC7D53-38AE-4E14-9D16-5C0AB081DB88}">
-  <dimension ref="A1:C22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DDC7D53-38AE-4E14-9D16-5C0AB081DB88}">
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" customWidth="1"/>
-    <col min="2" max="2" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" customWidth="1"/>
+    <col min="3" max="3" width="38" customWidth="1"/>
+    <col min="4" max="4" width="44.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -997,163 +1750,503 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="D4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E4" t="s">
+        <v>196</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E5" t="s">
+        <v>198</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D6" t="s">
+        <v>156</v>
+      </c>
+      <c r="E6" t="s">
+        <v>198</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D7" t="s">
+        <v>194</v>
+      </c>
+      <c r="E7" t="s">
+        <v>197</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+      <c r="C8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D8" t="s">
+        <v>184</v>
+      </c>
+      <c r="E8" t="s">
+        <v>197</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+      <c r="C9" t="s">
+        <v>169</v>
+      </c>
+      <c r="D9" t="s">
+        <v>204</v>
+      </c>
+      <c r="E9" t="s">
+        <v>197</v>
+      </c>
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>44</v>
       </c>
       <c r="B10" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>162</v>
+      </c>
+      <c r="D10" t="s">
+        <v>161</v>
+      </c>
+      <c r="E10" t="s">
+        <v>196</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>158</v>
+      </c>
+      <c r="C11" t="s">
+        <v>157</v>
+      </c>
+      <c r="D11" t="s">
+        <v>154</v>
+      </c>
+      <c r="E11" t="s">
+        <v>197</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" t="s">
+        <v>191</v>
+      </c>
+      <c r="D12" t="s">
+        <v>154</v>
+      </c>
+      <c r="E12" t="s">
+        <v>197</v>
+      </c>
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>164</v>
+      </c>
+      <c r="C13" t="s">
+        <v>165</v>
+      </c>
+      <c r="D13" t="s">
+        <v>154</v>
+      </c>
+      <c r="E13" t="s">
+        <v>197</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>48</v>
       </c>
       <c r="B14" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>190</v>
+      </c>
+      <c r="D14" t="s">
+        <v>154</v>
+      </c>
+      <c r="E14" t="s">
+        <v>197</v>
+      </c>
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C15" t="s">
+        <v>166</v>
+      </c>
+      <c r="D15" t="s">
+        <v>154</v>
+      </c>
+      <c r="E15" t="s">
+        <v>197</v>
+      </c>
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="B16" t="s">
+        <v>173</v>
+      </c>
+      <c r="C16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D16" t="s">
+        <v>154</v>
+      </c>
+      <c r="E16" t="s">
+        <v>197</v>
+      </c>
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="B17" t="s">
+        <v>171</v>
+      </c>
+      <c r="C17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D17" t="s">
+        <v>154</v>
+      </c>
+      <c r="E17" t="s">
+        <v>197</v>
+      </c>
+      <c r="F17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+      <c r="B18" t="s">
+        <v>181</v>
+      </c>
+      <c r="C18" t="s">
+        <v>182</v>
+      </c>
+      <c r="D18" t="s">
+        <v>178</v>
+      </c>
+      <c r="E18" t="s">
+        <v>197</v>
+      </c>
+      <c r="F18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+      <c r="B19" t="s">
+        <v>179</v>
+      </c>
+      <c r="C19" t="s">
+        <v>180</v>
+      </c>
+      <c r="D19" t="s">
+        <v>178</v>
+      </c>
+      <c r="E19" t="s">
+        <v>197</v>
+      </c>
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>201</v>
+      </c>
+      <c r="C20" t="s">
+        <v>162</v>
+      </c>
+      <c r="D20" t="s">
+        <v>170</v>
+      </c>
+      <c r="E20" t="s">
+        <v>196</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
+        <v>183</v>
+      </c>
+      <c r="C21" t="s">
+        <v>163</v>
+      </c>
+      <c r="D21" t="s">
+        <v>202</v>
+      </c>
+      <c r="E21" t="s">
+        <v>198</v>
+      </c>
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>187</v>
+      </c>
+      <c r="C22" t="s">
+        <v>188</v>
+      </c>
+      <c r="D22" t="s">
+        <v>203</v>
+      </c>
+      <c r="E22" t="s">
+        <v>199</v>
+      </c>
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" t="s">
+        <v>185</v>
+      </c>
+      <c r="C23" t="s">
+        <v>186</v>
+      </c>
+      <c r="D23" t="s">
+        <v>152</v>
+      </c>
+      <c r="E23" t="s">
+        <v>199</v>
+      </c>
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" t="s">
+        <v>183</v>
+      </c>
+      <c r="C24" t="s">
+        <v>189</v>
+      </c>
+      <c r="D24" t="s">
+        <v>153</v>
+      </c>
+      <c r="E24" t="s">
+        <v>199</v>
+      </c>
+      <c r="F24" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F24" xr:uid="{4CA2DF3C-A29E-4198-8908-251FC956AE4C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F24">
+    <sortCondition ref="D21"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE5D99A2-B987-4E19-A171-ABA2F3A75912}">
-  <dimension ref="A1:L13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE5D99A2-B987-4E19-A171-ABA2F3A75912}">
+  <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" customWidth="1"/>
     <col min="4" max="10" width="7.140625" customWidth="1"/>
+    <col min="15" max="15" width="56" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -1485,16 +2578,359 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="D15" t="s">
+        <v>219</v>
+      </c>
+      <c r="F15" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="C16" t="s">
+        <v>215</v>
+      </c>
+      <c r="D16" t="s">
+        <v>211</v>
+      </c>
+      <c r="E16" t="s">
+        <v>218</v>
+      </c>
+      <c r="F16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B17" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C17" t="s">
+        <v>215</v>
+      </c>
+      <c r="D17" t="s">
+        <v>211</v>
+      </c>
+      <c r="E17" t="s">
+        <v>218</v>
+      </c>
+      <c r="F17" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B18" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C18" t="s">
+        <v>212</v>
+      </c>
+      <c r="D18" t="s">
+        <v>211</v>
+      </c>
+      <c r="E18" t="s">
+        <v>218</v>
+      </c>
+      <c r="F18" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B19" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" t="s">
+        <v>214</v>
+      </c>
+      <c r="D19" t="s">
+        <v>211</v>
+      </c>
+      <c r="F19" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B20" s="27"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>149</v>
+      </c>
+      <c r="D21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B22" s="20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B23" s="11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B24" s="23" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B25" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="D25" s="22">
+        <v>47</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="N25" t="s">
+        <v>146</v>
+      </c>
+      <c r="O25" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B26" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="D26" s="21">
+        <v>45</v>
+      </c>
+      <c r="F26" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="N26" t="s">
+        <v>146</v>
+      </c>
+      <c r="O26" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B27" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C27" t="s">
+        <v>134</v>
+      </c>
+      <c r="D27">
+        <v>45</v>
+      </c>
+      <c r="E27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="N27" t="s">
+        <v>146</v>
+      </c>
+      <c r="O27" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B28" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C28" t="s">
+        <v>130</v>
+      </c>
+      <c r="D28">
+        <v>47</v>
+      </c>
+      <c r="E28" t="b">
+        <v>0</v>
+      </c>
+      <c r="F28" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="N28" t="s">
+        <v>146</v>
+      </c>
+      <c r="O28" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B29" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C29" t="s">
+        <v>127</v>
+      </c>
+      <c r="D29">
+        <v>47</v>
+      </c>
+      <c r="E29" t="b">
+        <v>1</v>
+      </c>
+      <c r="F29" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="N29" t="s">
+        <v>146</v>
+      </c>
+      <c r="O29" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="F30" s="21"/>
+      <c r="N30" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B31" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="F31" s="21"/>
+      <c r="N31" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B32" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C32" t="s">
+        <v>134</v>
+      </c>
+      <c r="D32">
+        <v>45</v>
+      </c>
+      <c r="F32" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="N32" t="s">
+        <v>146</v>
+      </c>
+      <c r="O32" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B33" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" t="s">
+        <v>130</v>
+      </c>
+      <c r="D33">
+        <v>47</v>
+      </c>
+      <c r="E33" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="F33" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="N33" t="s">
+        <v>146</v>
+      </c>
+      <c r="O33" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B34" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C34" t="s">
+        <v>127</v>
+      </c>
+      <c r="D34">
+        <v>47</v>
+      </c>
+      <c r="F34" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="N34" t="s">
+        <v>146</v>
+      </c>
+      <c r="O34" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F62BD8A-AB80-4EAF-ADD1-A729FC57348B}">
+  <dimension ref="D2"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="46.7109375" customWidth="1"/>
+    <col min="4" max="4" width="44" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF307F37-89F6-4478-B427-6D1C32C2CB55}">
   <dimension ref="B7:B32"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -1583,7 +3019,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{133B7AB1-EBB5-464D-9336-80F19EC6C35C}">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -1683,11 +3119,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1401EBAE-9336-4B4D-A642-B50D738A0A79}">
   <dimension ref="B12:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T26" sqref="T26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Misc Updates to comit
</commit_message>
<xml_diff>
--- a/BballMVC/_Documentation/BballMVC_Doc.xlsx
+++ b/BballMVC/_Documentation/BballMVC_Doc.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\wwwroot\Test\mrroot123\mrroot123\BballMVCproject\BballMVC\_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C7D841-03C3-4D29-B095-08A41E8FE55F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D7DC86-313D-4D56-B10A-EEC7F44814B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1575" yWindow="405" windowWidth="26835" windowHeight="14535" activeTab="2" xr2:uid="{03DA9A79-FE21-4B9D-9E56-4EA80CA75797}"/>
+    <workbookView xWindow="405" yWindow="150" windowWidth="26550" windowHeight="14670" activeTab="1" xr2:uid="{03DA9A79-FE21-4B9D-9E56-4EA80CA75797}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="3" r:id="rId1"/>
     <sheet name="Tables" sheetId="1" r:id="rId2"/>
     <sheet name="References" sheetId="2" r:id="rId3"/>
     <sheet name="DLLs" sheetId="7" r:id="rId4"/>
-    <sheet name="Adj Page" sheetId="4" r:id="rId5"/>
+    <sheet name="UI Adj Page" sheetId="4" r:id="rId5"/>
     <sheet name="Adj Point Pct" sheetId="5" r:id="rId6"/>
-    <sheet name="BoxScore Seed Screen" sheetId="6" r:id="rId7"/>
+    <sheet name="Pt Value Analysis" sheetId="8" r:id="rId7"/>
+    <sheet name="BoxScore Seed Screen" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tables!$A$1:$F$24</definedName>
@@ -89,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="235">
   <si>
     <t>Table</t>
   </si>
@@ -224,9 +225,6 @@
   </si>
   <si>
     <t>Lines</t>
-  </si>
-  <si>
-    <t>MatchupsResults</t>
   </si>
   <si>
     <t>ParmTable</t>
@@ -907,9 +905,6 @@
     <t>variable</t>
   </si>
   <si>
-    <t>uspCalcTM - step 2 - uspInsertMatchupResults</t>
-  </si>
-  <si>
     <t>uspCalcTM - step 2 - uspQueryCalcTeamStrength</t>
   </si>
   <si>
@@ -984,6 +979,54 @@
       </rPr>
       <t>\mrroot123\BballMVCproject\</t>
     </r>
+  </si>
+  <si>
+    <t>Fix Excluded BxSc s</t>
+  </si>
+  <si>
+    <t>Convert Adjs - no ranges</t>
+  </si>
+  <si>
+    <t>Handle Postponed games</t>
+  </si>
+  <si>
+    <t>Half Line analysis</t>
+  </si>
+  <si>
+    <t>Get Half Lines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adjustments - Recent History, OT, TV, </t>
+  </si>
+  <si>
+    <t>Calc Threshold via Volity</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>#usp_Backup_00TTI_LeagueScores.sql</t>
+  </si>
+  <si>
+    <t>verfiy</t>
+  </si>
+  <si>
+    <t>Verify_Boxscores.sql</t>
+  </si>
+  <si>
+    <t>Lg, TV, OT adjs per TEAM</t>
+  </si>
+  <si>
+    <t>0Seq</t>
+  </si>
+  <si>
+    <t>TodaysMatchupsResults</t>
+  </si>
+  <si>
+    <t>uspCalcTM - step 2 - uspInsertTodaysMatchupsResults</t>
   </si>
 </sst>
 </file>
@@ -1119,7 +1162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1133,7 +1176,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -1171,6 +1213,9 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1676,58 +1721,181 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80042610-4475-439E-8D8A-B99F3A7253D1}">
-  <dimension ref="A1:C4"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:H15"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>232</v>
+      </c>
+      <c r="B1" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="D1" s="29" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="26">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="30">
         <v>43989</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="E2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="25">
+        <v>43989</v>
+      </c>
+      <c r="C3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D3" t="s">
+        <v>204</v>
+      </c>
+      <c r="E3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2.1</v>
+      </c>
+      <c r="B4" s="25">
+        <v>43989</v>
+      </c>
+      <c r="D4" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C3" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>207</v>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="25">
+        <v>43991</v>
+      </c>
+      <c r="C5" t="s">
+        <v>227</v>
+      </c>
+      <c r="D5" t="s">
+        <v>219</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="25">
+        <v>43991</v>
+      </c>
+      <c r="C6" t="s">
+        <v>229</v>
+      </c>
+      <c r="D6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D7" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4.2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4.3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10" s="25">
+        <v>44084</v>
+      </c>
+      <c r="D10" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>6.1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F12">
+    <sortCondition ref="A2:A12"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DDC7D53-38AE-4E14-9D16-5C0AB081DB88}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1750,14 +1918,14 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
-        <v>151</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>195</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>200</v>
+      <c r="D1" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1765,16 +1933,16 @@
         <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -1791,10 +1959,10 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -1811,10 +1979,10 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
@@ -1831,10 +1999,10 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
@@ -1845,16 +2013,16 @@
         <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
@@ -1865,16 +2033,16 @@
         <v>41</v>
       </c>
       <c r="B7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C7" t="s">
         <v>192</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>193</v>
       </c>
-      <c r="D7" t="s">
-        <v>194</v>
-      </c>
       <c r="E7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
@@ -1882,19 +2050,19 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
@@ -1902,19 +2070,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C9" t="s">
         <v>168</v>
       </c>
-      <c r="C9" t="s">
-        <v>169</v>
-      </c>
       <c r="D9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -1925,16 +2093,16 @@
         <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F10" t="b">
         <v>1</v>
@@ -1945,16 +2113,16 @@
         <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
@@ -1965,16 +2133,16 @@
         <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
@@ -1982,19 +2150,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
+        <v>163</v>
+      </c>
+      <c r="C13" t="s">
         <v>164</v>
       </c>
-      <c r="C13" t="s">
-        <v>165</v>
-      </c>
       <c r="D13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F13" t="b">
         <v>0</v>
@@ -2002,19 +2170,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
@@ -2022,19 +2190,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
@@ -2042,19 +2210,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16" t="s">
+        <v>172</v>
+      </c>
+      <c r="C16" t="s">
         <v>173</v>
       </c>
-      <c r="C16" t="s">
-        <v>174</v>
-      </c>
       <c r="D16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F16" t="b">
         <v>0</v>
@@ -2062,19 +2230,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s">
+        <v>170</v>
+      </c>
+      <c r="C17" t="s">
         <v>171</v>
       </c>
-      <c r="C17" t="s">
-        <v>172</v>
-      </c>
       <c r="D17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F17" t="b">
         <v>0</v>
@@ -2082,19 +2250,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B18" t="s">
+        <v>180</v>
+      </c>
+      <c r="C18" t="s">
         <v>181</v>
       </c>
-      <c r="C18" t="s">
-        <v>182</v>
-      </c>
       <c r="D18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
@@ -2102,19 +2270,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>176</v>
+      </c>
+      <c r="B19" t="s">
+        <v>178</v>
+      </c>
+      <c r="C19" t="s">
+        <v>179</v>
+      </c>
+      <c r="D19" t="s">
         <v>177</v>
       </c>
-      <c r="B19" t="s">
-        <v>179</v>
-      </c>
-      <c r="C19" t="s">
-        <v>180</v>
-      </c>
-      <c r="D19" t="s">
-        <v>178</v>
-      </c>
       <c r="E19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
@@ -2122,19 +2290,19 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F20" t="b">
         <v>1</v>
@@ -2142,19 +2310,19 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>233</v>
       </c>
       <c r="B21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D21" t="s">
-        <v>202</v>
+        <v>234</v>
       </c>
       <c r="E21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F21" t="b">
         <v>1</v>
@@ -2162,19 +2330,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
+        <v>186</v>
+      </c>
+      <c r="C22" t="s">
         <v>187</v>
       </c>
-      <c r="C22" t="s">
-        <v>188</v>
-      </c>
       <c r="D22" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F22" t="b">
         <v>1</v>
@@ -2182,19 +2350,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B23" t="s">
+        <v>184</v>
+      </c>
+      <c r="C23" t="s">
         <v>185</v>
       </c>
-      <c r="C23" t="s">
-        <v>186</v>
-      </c>
       <c r="D23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E23" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F23" t="b">
         <v>1</v>
@@ -2202,19 +2370,19 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E24" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F24" t="b">
         <v>1</v>
@@ -2233,9 +2401,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE5D99A2-B987-4E19-A171-ABA2F3A75912}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N22" sqref="N22"/>
     </sheetView>
@@ -2579,162 +2748,162 @@
       <c r="L13" s="5"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="D15" t="s">
+        <v>217</v>
+      </c>
+      <c r="F15" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C16" t="s">
+        <v>213</v>
+      </c>
+      <c r="D16" t="s">
+        <v>209</v>
+      </c>
+      <c r="E16" t="s">
         <v>216</v>
       </c>
-      <c r="D15" t="s">
-        <v>219</v>
-      </c>
-      <c r="F15" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="11" t="s">
+      <c r="F16" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" t="s">
+        <v>213</v>
+      </c>
+      <c r="D17" t="s">
+        <v>209</v>
+      </c>
+      <c r="E17" t="s">
+        <v>216</v>
+      </c>
+      <c r="F17" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B18" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" t="s">
+        <v>210</v>
+      </c>
+      <c r="D18" t="s">
+        <v>209</v>
+      </c>
+      <c r="E18" t="s">
+        <v>216</v>
+      </c>
+      <c r="F18" t="s">
         <v>211</v>
       </c>
-      <c r="C16" t="s">
-        <v>215</v>
-      </c>
-      <c r="D16" t="s">
-        <v>211</v>
-      </c>
-      <c r="E16" t="s">
-        <v>218</v>
-      </c>
-      <c r="F16" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="C17" t="s">
-        <v>215</v>
-      </c>
-      <c r="D17" t="s">
-        <v>211</v>
-      </c>
-      <c r="E17" t="s">
-        <v>218</v>
-      </c>
-      <c r="F17" t="s">
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B19" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D19" t="s">
+        <v>209</v>
+      </c>
+      <c r="F19" t="s">
         <v>212</v>
       </c>
-      <c r="D18" t="s">
-        <v>211</v>
-      </c>
-      <c r="E18" t="s">
-        <v>218</v>
-      </c>
-      <c r="F18" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="C19" t="s">
-        <v>214</v>
-      </c>
-      <c r="D19" t="s">
-        <v>211</v>
-      </c>
-      <c r="F19" t="s">
-        <v>214</v>
-      </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B20" s="27"/>
+      <c r="B20" s="26"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
+        <v>148</v>
+      </c>
+      <c r="D21" t="s">
         <v>149</v>
       </c>
-      <c r="D21" t="s">
-        <v>150</v>
-      </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B22" s="20" t="s">
-        <v>137</v>
+      <c r="B22" s="19" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B24" s="22" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B24" s="23" t="s">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B25" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" s="21" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B25" s="11" t="s">
+      <c r="D25" s="21">
+        <v>47</v>
+      </c>
+      <c r="F25" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="N25" t="s">
+        <v>145</v>
+      </c>
+      <c r="O25" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B26" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C26" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="C25" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="D25" s="22">
-        <v>47</v>
-      </c>
-      <c r="F25" s="21" t="s">
-        <v>220</v>
-      </c>
-      <c r="N25" t="s">
-        <v>146</v>
-      </c>
-      <c r="O25" t="s">
+      <c r="D26" s="20">
+        <v>45</v>
+      </c>
+      <c r="F26" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="Q25" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B26" s="11" t="s">
+      <c r="N26" t="s">
+        <v>145</v>
+      </c>
+      <c r="O26" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q26" t="s">
         <v>122</v>
       </c>
-      <c r="C26" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="D26" s="21">
-        <v>45</v>
-      </c>
-      <c r="F26" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="N26" t="s">
-        <v>146</v>
-      </c>
-      <c r="O26" t="s">
-        <v>141</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>123</v>
-      </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C27" t="s">
         <v>133</v>
-      </c>
-      <c r="C27" t="s">
-        <v>134</v>
       </c>
       <c r="D27">
         <v>45</v>
@@ -2742,25 +2911,25 @@
       <c r="E27" t="b">
         <v>1</v>
       </c>
-      <c r="F27" s="21" t="s">
-        <v>138</v>
+      <c r="F27" s="20" t="s">
+        <v>137</v>
       </c>
       <c r="N27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Q27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C28" t="s">
         <v>129</v>
-      </c>
-      <c r="C28" t="s">
-        <v>130</v>
       </c>
       <c r="D28">
         <v>47</v>
@@ -2768,25 +2937,25 @@
       <c r="E28" t="b">
         <v>0</v>
       </c>
-      <c r="F28" s="21" t="s">
-        <v>138</v>
+      <c r="F28" s="20" t="s">
+        <v>137</v>
       </c>
       <c r="N28" t="s">
-        <v>146</v>
-      </c>
-      <c r="O28" s="12" t="s">
-        <v>143</v>
+        <v>145</v>
+      </c>
+      <c r="O28" s="11" t="s">
+        <v>142</v>
       </c>
       <c r="Q28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B29" s="11" t="s">
-        <v>125</v>
+      <c r="B29" s="10" t="s">
+        <v>124</v>
       </c>
       <c r="C29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D29">
         <v>47</v>
@@ -2794,104 +2963,104 @@
       <c r="E29" t="b">
         <v>1</v>
       </c>
-      <c r="F29" s="21" t="s">
-        <v>138</v>
+      <c r="F29" s="20" t="s">
+        <v>137</v>
       </c>
       <c r="N29" t="s">
+        <v>145</v>
+      </c>
+      <c r="O29" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="F30" s="20"/>
+      <c r="N30" t="s">
         <v>146</v>
       </c>
-      <c r="O29" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="F30" s="21"/>
-      <c r="N30" t="s">
-        <v>147</v>
-      </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="F31" s="20"/>
+      <c r="N31" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B32" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="F31" s="21"/>
-      <c r="N31" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B32" s="11" t="s">
+      <c r="C32" t="s">
         <v>133</v>
-      </c>
-      <c r="C32" t="s">
-        <v>134</v>
       </c>
       <c r="D32">
         <v>45</v>
       </c>
-      <c r="F32" s="21" t="s">
-        <v>138</v>
+      <c r="F32" s="20" t="s">
+        <v>137</v>
       </c>
       <c r="N32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Q32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C33" t="s">
         <v>129</v>
-      </c>
-      <c r="C33" t="s">
-        <v>130</v>
       </c>
       <c r="D33">
         <v>47</v>
       </c>
-      <c r="E33" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="F33" s="21" t="s">
-        <v>138</v>
+      <c r="E33" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>137</v>
       </c>
       <c r="N33" t="s">
-        <v>146</v>
-      </c>
-      <c r="O33" s="12" t="s">
         <v>145</v>
       </c>
+      <c r="O33" s="11" t="s">
+        <v>144</v>
+      </c>
       <c r="Q33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="34" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B34" s="11" t="s">
-        <v>125</v>
+      <c r="B34" s="10" t="s">
+        <v>124</v>
       </c>
       <c r="C34" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D34">
         <v>47</v>
       </c>
-      <c r="F34" s="21" t="s">
-        <v>138</v>
+      <c r="F34" s="20" t="s">
+        <v>137</v>
       </c>
       <c r="N34" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="Q34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2903,6 +3072,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F62BD8A-AB80-4EAF-ADD1-A729FC57348B}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="D2"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -2916,7 +3086,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="23" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2928,9 +3098,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF307F37-89F6-4478-B427-6D1C32C2CB55}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="B7:B32"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -2940,77 +3111,77 @@
   </cols>
   <sheetData>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="10" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B15" s="10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="11" t="s">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="10" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="11" t="s">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="10" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="11" t="s">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="13" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="14" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="15" t="s">
-        <v>71</v>
+      <c r="B29" s="14" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="12"/>
+      <c r="B32" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3021,36 +3192,37 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{133B7AB1-EBB5-464D-9336-80F19EC6C35C}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>73</v>
-      </c>
-      <c r="D1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>74</v>
       </c>
       <c r="B2">
         <v>-3</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>75</v>
+      <c r="A3" s="15" t="s">
+        <v>74</v>
       </c>
       <c r="B3">
         <v>20</v>
@@ -3061,8 +3233,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
-        <v>76</v>
+      <c r="A4" s="15" t="s">
+        <v>75</v>
       </c>
       <c r="B4">
         <v>25</v>
@@ -3073,8 +3245,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>77</v>
+      <c r="A5" s="15" t="s">
+        <v>76</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -3085,16 +3257,16 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>83</v>
+      <c r="A7" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>80</v>
+      <c r="A8" s="15" t="s">
+        <v>79</v>
       </c>
       <c r="B8">
         <f>B3 + B4 * 2 + B5 * 3</f>
@@ -3106,8 +3278,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
-        <v>81</v>
+      <c r="A10" s="15" t="s">
+        <v>80</v>
       </c>
       <c r="B10">
         <f xml:space="preserve"> 1 + (B2 / B8)</f>
@@ -3120,7 +3292,153 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C17B75FB-3788-4C0A-A5BD-D95698756B72}">
+  <sheetPr codeName="Sheet7"/>
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>-4</v>
+      </c>
+      <c r="B1">
+        <v>40.6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>-3</v>
+      </c>
+      <c r="B2">
+        <v>43.12</v>
+      </c>
+      <c r="C2">
+        <f>B2-B1</f>
+        <v>2.519999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>-2</v>
+      </c>
+      <c r="B3">
+        <v>45.51</v>
+      </c>
+      <c r="C3">
+        <f>B3-B2</f>
+        <v>2.3900000000000006</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A9" si="0">A3+1</f>
+        <v>-1</v>
+      </c>
+      <c r="B4">
+        <v>47.8</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C9" si="1">B4-B3</f>
+        <v>2.2899999999999991</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>50.36</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>2.5600000000000023</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>53</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>2.6400000000000006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>55.23</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>2.2299999999999969</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>57.49</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>2.2600000000000051</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>59.76</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>2.269999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="28">
+        <f>AVERAGE(C2:C9)</f>
+        <v>2.3949999999999996</v>
+      </c>
+      <c r="D10" s="28">
+        <f>AVERAGE(C4:C7)</f>
+        <v>2.4299999999999997</v>
+      </c>
+      <c r="E10" s="28">
+        <f>AVERAGE(C4:C6)</f>
+        <v>2.4966666666666675</v>
+      </c>
+      <c r="F10" s="28">
+        <f>(B8-B2)/6</f>
+        <v>2.3950000000000009</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1401EBAE-9336-4B4D-A642-B50D738A0A79}">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="B12:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3139,161 +3457,161 @@
     <row r="16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="18" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="19" t="s">
+      <c r="C20" s="19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D21" s="16" t="s">
         <v>86</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D21" s="17" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="18" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="19" t="s">
+      <c r="C24" s="19" t="s">
         <v>89</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="C41" s="20" t="s">
-        <v>109</v>
+      <c r="B41" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rotation - Added Season Info columns
</commit_message>
<xml_diff>
--- a/BballMVC/_Documentation/BballMVC_Doc.xlsx
+++ b/BballMVC/_Documentation/BballMVC_Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\wwwroot\Test\mrroot123\mrroot123\BballMVCproject\BballMVC\_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D7DC86-313D-4D56-B10A-EEC7F44814B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52ECBF3-B5D5-4852-B53B-A2D226089CD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="405" yWindow="150" windowWidth="26550" windowHeight="14670" activeTab="1" xr2:uid="{03DA9A79-FE21-4B9D-9E56-4EA80CA75797}"/>
+    <workbookView xWindow="405" yWindow="150" windowWidth="26550" windowHeight="14670" xr2:uid="{03DA9A79-FE21-4B9D-9E56-4EA80CA75797}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="3" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="236">
   <si>
     <t>Table</t>
   </si>
@@ -1027,6 +1027,9 @@
   </si>
   <si>
     <t>uspCalcTM - step 2 - uspInsertTodaysMatchupsResults</t>
+  </si>
+  <si>
+    <t>Rotation - add Season &amp; SubSeason</t>
   </si>
 </sst>
 </file>
@@ -1722,11 +1725,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80042610-4475-439E-8D8A-B99F3A7253D1}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1880,6 +1883,11 @@
         <v>223</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>235</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F12">
     <sortCondition ref="A2:A12"/>
@@ -1893,7 +1901,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
     </sheetView>

</xml_diff>

<commit_message>
Updated uspCalcTMs w Open TL
</commit_message>
<xml_diff>
--- a/BballMVC/_Documentation/BballMVC_Doc.xlsx
+++ b/BballMVC/_Documentation/BballMVC_Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\wwwroot\Test\mrroot123\mrroot123\BballMVCproject\BballMVC\_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1F579A-E11A-44B9-AF6B-659F83678B79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F71C96-5524-4DA3-9E2D-7B1A9CBD1E68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30315" yWindow="1515" windowWidth="21600" windowHeight="11835" activeTab="2" xr2:uid="{03DA9A79-FE21-4B9D-9E56-4EA80CA75797}"/>
+    <workbookView xWindow="480" yWindow="855" windowWidth="24150" windowHeight="13470" activeTab="1" xr2:uid="{03DA9A79-FE21-4B9D-9E56-4EA80CA75797}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="3" r:id="rId1"/>
@@ -22,10 +22,9 @@
     <sheet name="Pt Value Analysis" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tables!$A$1:$F$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tables!$B$1:$G$25</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +39,7 @@
     <author>Keith</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{E9F86DB3-32F0-4C4D-B010-4B9243F98F96}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{E9F86DB3-32F0-4C4D-B010-4B9243F98F96}">
       <text>
         <r>
           <rPr>
@@ -84,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="224">
   <si>
     <t>Table</t>
   </si>
@@ -794,9 +793,6 @@
     <t>Today</t>
   </si>
   <si>
-    <t>GameDate</t>
-  </si>
-  <si>
     <t>variable</t>
   </si>
   <si>
@@ -1022,12 +1018,43 @@
   <si>
     <t xml:space="preserve">         // 08/30/2020 removed Unity Container</t>
   </si>
+  <si>
+    <t>Bball
+Start Date</t>
+  </si>
+  <si>
+    <t>Bball
+ Rows</t>
+  </si>
+  <si>
+    <t>SqlX
+Start Date</t>
+  </si>
+  <si>
+    <t>SqlX
+Rows</t>
+  </si>
+  <si>
+    <t>Game
+Date</t>
+  </si>
+  <si>
+    <t>PROD
+Start Date</t>
+  </si>
+  <si>
+    <t>PROD
+Rows</t>
+  </si>
+  <si>
+    <t>Sql2012</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1084,6 +1111,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1105,7 +1140,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1152,11 +1187,122 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1206,6 +1352,32 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1681,13 +1853,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>37</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D1" s="27" t="s">
         <v>38</v>
@@ -1701,13 +1873,13 @@
         <v>43989</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1721,10 +1893,10 @@
         <v>113</v>
       </c>
       <c r="D3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1735,7 +1907,7 @@
         <v>43989</v>
       </c>
       <c r="D4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1746,16 +1918,16 @@
         <v>43991</v>
       </c>
       <c r="C5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E5">
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1766,10 +1938,10 @@
         <v>43991</v>
       </c>
       <c r="C6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1777,7 +1949,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1785,7 +1957,7 @@
         <v>4.2</v>
       </c>
       <c r="D8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1793,7 +1965,7 @@
         <v>4.3</v>
       </c>
       <c r="D9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1804,7 +1976,7 @@
         <v>44084</v>
       </c>
       <c r="D10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1812,7 +1984,7 @@
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1820,7 +1992,7 @@
         <v>6.1</v>
       </c>
       <c r="D12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1828,20 +2000,20 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -1856,528 +2028,734 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DDC7D53-38AE-4E14-9D16-5C0AB081DB88}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
-    <col min="2" max="2" width="46.28515625" customWidth="1"/>
-    <col min="3" max="3" width="38" customWidth="1"/>
-    <col min="4" max="4" width="44.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="38" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="44.5703125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="E1" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="F1" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G1" s="31" t="s">
+        <v>220</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="J1" s="30" t="s">
+        <v>218</v>
+      </c>
+      <c r="K1" s="32" t="s">
+        <v>219</v>
+      </c>
+      <c r="L1" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="M1" s="29" t="s">
+        <v>222</v>
+      </c>
+      <c r="N1" s="30" t="s">
+        <v>223</v>
+      </c>
+      <c r="O1" s="30" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" s="44">
+        <v>43466</v>
+      </c>
+      <c r="I2" s="36">
+        <v>6077</v>
+      </c>
+      <c r="J2" s="42">
+        <v>43466</v>
+      </c>
+      <c r="K2" s="36">
+        <v>6080</v>
+      </c>
+      <c r="L2" s="42">
+        <v>43466</v>
+      </c>
+      <c r="M2" s="37">
+        <v>6076</v>
+      </c>
+      <c r="N2" s="35">
+        <v>39449</v>
+      </c>
+      <c r="O2">
+        <v>49524</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3" t="s">
+        <v>164</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" s="45">
+        <v>40087</v>
+      </c>
+      <c r="I3" s="38">
+        <v>28500</v>
+      </c>
+      <c r="J3" s="34">
+        <v>40087</v>
+      </c>
+      <c r="K3" s="38">
+        <v>28468</v>
+      </c>
+      <c r="L3" s="34">
+        <v>40087</v>
+      </c>
+      <c r="M3" s="39">
+        <v>28502</v>
+      </c>
+      <c r="N3" s="35">
+        <v>40087</v>
+      </c>
+      <c r="O3">
+        <v>28200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" t="s">
+        <v>122</v>
+      </c>
+      <c r="F4" t="s">
+        <v>164</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" s="45">
+        <v>43370</v>
+      </c>
+      <c r="I4" s="38">
+        <v>4594</v>
+      </c>
+      <c r="J4" s="34">
+        <v>43370</v>
+      </c>
+      <c r="K4" s="38">
+        <v>4608</v>
+      </c>
+      <c r="L4" s="34">
+        <v>43370</v>
+      </c>
+      <c r="M4" s="39">
+        <v>4592</v>
+      </c>
+      <c r="N4" s="35">
+        <v>43370</v>
+      </c>
+      <c r="O4">
+        <v>4560</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>122</v>
+      </c>
+      <c r="F5" t="s">
+        <v>162</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="46">
+        <v>40893</v>
+      </c>
+      <c r="I5" s="40">
+        <v>23542</v>
+      </c>
+      <c r="J5" s="43">
+        <v>40893</v>
+      </c>
+      <c r="K5" s="40">
+        <v>23510</v>
+      </c>
+      <c r="L5" s="43">
+        <v>40893</v>
+      </c>
+      <c r="M5" s="41">
+        <v>23540</v>
+      </c>
+      <c r="N5" s="35">
+        <v>40893</v>
+      </c>
+      <c r="O5">
+        <v>23210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F6" t="s">
+        <v>163</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="L6" s="33"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>158</v>
+      </c>
+      <c r="D7" t="s">
+        <v>159</v>
+      </c>
+      <c r="E7" t="s">
+        <v>160</v>
+      </c>
+      <c r="F7" t="s">
+        <v>163</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="L7" s="33"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" t="s">
+        <v>145</v>
+      </c>
+      <c r="D8" t="s">
+        <v>146</v>
+      </c>
+      <c r="E8" t="s">
+        <v>144</v>
+      </c>
+      <c r="F8" t="s">
+        <v>163</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="L8" s="33"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>122</v>
+      </c>
+      <c r="F9" t="s">
+        <v>162</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="L9" s="33"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E10" t="s">
+        <v>120</v>
+      </c>
+      <c r="F10" t="s">
+        <v>163</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="L10" s="33"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E11" t="s">
+        <v>127</v>
+      </c>
+      <c r="F11" t="s">
+        <v>162</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="L11" s="33"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
+        <v>130</v>
+      </c>
+      <c r="D12" t="s">
+        <v>131</v>
+      </c>
+      <c r="E12" t="s">
+        <v>120</v>
+      </c>
+      <c r="F12" t="s">
+        <v>163</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="L12" s="33"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>150</v>
+      </c>
+      <c r="D13" t="s">
+        <v>141</v>
+      </c>
+      <c r="E13" t="s">
+        <v>150</v>
+      </c>
+      <c r="F13" t="s">
+        <v>163</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="L13" s="33"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" t="s">
+        <v>147</v>
+      </c>
+      <c r="D14" t="s">
+        <v>148</v>
+      </c>
+      <c r="E14" t="s">
+        <v>144</v>
+      </c>
+      <c r="F14" t="s">
+        <v>163</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" s="33"/>
+      <c r="J14" s="33"/>
+      <c r="L14" s="33"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" t="s">
+        <v>156</v>
+      </c>
+      <c r="E15" t="s">
+        <v>120</v>
+      </c>
+      <c r="F15" t="s">
+        <v>163</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="33"/>
+      <c r="J15" s="33"/>
+      <c r="L15" s="33"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
+        <v>133</v>
+      </c>
+      <c r="D16" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" t="s">
+        <v>120</v>
+      </c>
+      <c r="F16" t="s">
+        <v>163</v>
+      </c>
+      <c r="G16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" s="33"/>
+      <c r="J16" s="33"/>
+      <c r="L16" s="33"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D17" t="s">
+        <v>135</v>
+      </c>
+      <c r="E17" t="s">
+        <v>168</v>
+      </c>
+      <c r="F17" t="s">
+        <v>163</v>
+      </c>
+      <c r="G17" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" s="33"/>
+      <c r="J17" s="33"/>
+      <c r="L17" s="33"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
+        <v>151</v>
+      </c>
+      <c r="D18" t="s">
+        <v>152</v>
+      </c>
+      <c r="E18" t="s">
+        <v>118</v>
+      </c>
+      <c r="F18" t="s">
+        <v>165</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="L18" s="33"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" t="s">
+        <v>153</v>
+      </c>
+      <c r="D19" t="s">
+        <v>154</v>
+      </c>
+      <c r="E19" t="s">
         <v>167</v>
       </c>
-      <c r="C2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F19" t="s">
+        <v>165</v>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" s="33"/>
+      <c r="J19" s="33"/>
+      <c r="L19" s="33"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" t="s">
+        <v>149</v>
+      </c>
+      <c r="D20" t="s">
+        <v>155</v>
+      </c>
+      <c r="E20" t="s">
+        <v>119</v>
+      </c>
+      <c r="F20" t="s">
+        <v>165</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" s="33"/>
+      <c r="J20" s="33"/>
+      <c r="L20" s="33"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>199</v>
+      </c>
+      <c r="C21" t="s">
+        <v>149</v>
+      </c>
+      <c r="D21" t="s">
+        <v>129</v>
+      </c>
+      <c r="E21" t="s">
+        <v>200</v>
+      </c>
+      <c r="F21" t="s">
+        <v>164</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" s="33"/>
+      <c r="J21" s="33"/>
+      <c r="L21" s="33"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" t="s">
+        <v>166</v>
+      </c>
+      <c r="D22" t="s">
+        <v>128</v>
+      </c>
+      <c r="E22" t="s">
+        <v>136</v>
+      </c>
+      <c r="F22" t="s">
         <v>162</v>
       </c>
-      <c r="F2" t="b">
+      <c r="G22" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="H22" s="33"/>
+      <c r="J22" s="33"/>
+      <c r="L22" s="33"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" t="s">
+        <v>139</v>
+      </c>
+      <c r="D23" t="s">
+        <v>140</v>
+      </c>
+      <c r="E23" t="s">
         <v>120</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F23" t="s">
         <v>163</v>
       </c>
-      <c r="F3" t="b">
+      <c r="G23" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" t="s">
-        <v>158</v>
-      </c>
-      <c r="C4" t="s">
-        <v>159</v>
-      </c>
-      <c r="D4" t="s">
-        <v>160</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="H23" s="33"/>
+      <c r="J23" s="33"/>
+      <c r="L23" s="33"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" t="s">
+        <v>137</v>
+      </c>
+      <c r="D24" t="s">
+        <v>138</v>
+      </c>
+      <c r="E24" t="s">
+        <v>120</v>
+      </c>
+      <c r="F24" t="s">
         <v>163</v>
       </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>143</v>
-      </c>
-      <c r="B5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C5" t="s">
-        <v>146</v>
-      </c>
-      <c r="D5" t="s">
-        <v>144</v>
-      </c>
-      <c r="E5" t="s">
-        <v>163</v>
-      </c>
-      <c r="F5" t="b">
+      <c r="G24" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>122</v>
-      </c>
-      <c r="E6" t="s">
-        <v>164</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" t="s">
-        <v>126</v>
-      </c>
-      <c r="D7" t="s">
-        <v>122</v>
-      </c>
-      <c r="E7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s">
-        <v>122</v>
-      </c>
-      <c r="E8" t="s">
-        <v>162</v>
-      </c>
-      <c r="F8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" t="s">
-        <v>157</v>
-      </c>
-      <c r="D9" t="s">
-        <v>120</v>
-      </c>
-      <c r="E9" t="s">
-        <v>163</v>
-      </c>
-      <c r="F9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" t="s">
-        <v>128</v>
-      </c>
-      <c r="D10" t="s">
-        <v>127</v>
-      </c>
-      <c r="E10" t="s">
-        <v>162</v>
-      </c>
-      <c r="F10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" t="s">
-        <v>130</v>
-      </c>
-      <c r="C11" t="s">
-        <v>131</v>
-      </c>
-      <c r="D11" t="s">
-        <v>120</v>
-      </c>
-      <c r="E11" t="s">
-        <v>163</v>
-      </c>
-      <c r="F11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" t="s">
-        <v>150</v>
-      </c>
-      <c r="C12" t="s">
-        <v>141</v>
-      </c>
-      <c r="D12" t="s">
-        <v>150</v>
-      </c>
-      <c r="E12" t="s">
-        <v>163</v>
-      </c>
-      <c r="F12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>142</v>
-      </c>
-      <c r="B13" t="s">
-        <v>147</v>
-      </c>
-      <c r="C13" t="s">
-        <v>148</v>
-      </c>
-      <c r="D13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E13" t="s">
-        <v>163</v>
-      </c>
-      <c r="F13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" t="s">
-        <v>122</v>
-      </c>
-      <c r="E14" t="s">
-        <v>162</v>
-      </c>
-      <c r="F14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" t="s">
-        <v>156</v>
-      </c>
-      <c r="D15" t="s">
-        <v>120</v>
-      </c>
-      <c r="E15" t="s">
-        <v>163</v>
-      </c>
-      <c r="F15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" t="s">
-        <v>133</v>
-      </c>
-      <c r="C16" t="s">
-        <v>132</v>
-      </c>
-      <c r="D16" t="s">
-        <v>120</v>
-      </c>
-      <c r="E16" t="s">
-        <v>163</v>
-      </c>
-      <c r="F16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" t="s">
-        <v>134</v>
-      </c>
-      <c r="C17" t="s">
-        <v>135</v>
-      </c>
-      <c r="D17" t="s">
-        <v>169</v>
-      </c>
-      <c r="E17" t="s">
-        <v>163</v>
-      </c>
-      <c r="F17" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" t="s">
-        <v>151</v>
-      </c>
-      <c r="C18" t="s">
-        <v>152</v>
-      </c>
-      <c r="D18" t="s">
-        <v>118</v>
-      </c>
-      <c r="E18" t="s">
-        <v>165</v>
-      </c>
-      <c r="F18" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" t="s">
-        <v>153</v>
-      </c>
-      <c r="C19" t="s">
-        <v>154</v>
-      </c>
-      <c r="D19" t="s">
-        <v>168</v>
-      </c>
-      <c r="E19" t="s">
-        <v>165</v>
-      </c>
-      <c r="F19" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" t="s">
-        <v>149</v>
-      </c>
-      <c r="C20" t="s">
-        <v>155</v>
-      </c>
-      <c r="D20" t="s">
-        <v>119</v>
-      </c>
-      <c r="E20" t="s">
-        <v>165</v>
-      </c>
-      <c r="F20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>200</v>
-      </c>
-      <c r="B21" t="s">
-        <v>149</v>
-      </c>
-      <c r="C21" t="s">
-        <v>129</v>
-      </c>
-      <c r="D21" t="s">
-        <v>201</v>
-      </c>
-      <c r="E21" t="s">
-        <v>164</v>
-      </c>
-      <c r="F21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" t="s">
-        <v>167</v>
-      </c>
-      <c r="C22" t="s">
-        <v>128</v>
-      </c>
-      <c r="D22" t="s">
-        <v>136</v>
-      </c>
-      <c r="E22" t="s">
-        <v>162</v>
-      </c>
-      <c r="F22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" t="s">
-        <v>139</v>
-      </c>
-      <c r="C23" t="s">
-        <v>140</v>
-      </c>
-      <c r="D23" t="s">
-        <v>120</v>
-      </c>
-      <c r="E23" t="s">
-        <v>163</v>
-      </c>
-      <c r="F23" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" t="s">
-        <v>137</v>
-      </c>
-      <c r="C24" t="s">
-        <v>138</v>
-      </c>
-      <c r="D24" t="s">
-        <v>120</v>
-      </c>
-      <c r="E24" t="s">
-        <v>163</v>
-      </c>
-      <c r="F24" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>203</v>
-      </c>
-      <c r="C25" t="s">
-        <v>205</v>
+      <c r="H24" s="33"/>
+      <c r="J24" s="33"/>
+      <c r="L24" s="33"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>202</v>
       </c>
       <c r="D25" t="s">
         <v>204</v>
       </c>
       <c r="E25" t="s">
+        <v>203</v>
+      </c>
+      <c r="F25" t="s">
         <v>163</v>
       </c>
-      <c r="F25" t="b">
+      <c r="G25" t="b">
         <v>0</v>
       </c>
+      <c r="H25" s="33"/>
+      <c r="J25" s="33"/>
+      <c r="L25" s="33"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H26" s="33"/>
+      <c r="J26" s="33"/>
+      <c r="L26" s="33"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F24" xr:uid="{4CA2DF3C-A29E-4198-8908-251FC956AE4C}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F24">
-      <sortCondition ref="A4"/>
+  <autoFilter ref="B1:G25" xr:uid="{4CA2DF3C-A29E-4198-8908-251FC956AE4C}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:G24">
+      <sortCondition ref="B4"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F24">
-    <sortCondition ref="D21"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M25">
+    <sortCondition ref="A4"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2390,7 +2768,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
     </sheetView>
@@ -2735,33 +3113,33 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C15" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="D15" t="s">
+        <v>183</v>
+      </c>
+      <c r="F15" t="s">
         <v>181</v>
-      </c>
-      <c r="D15" t="s">
-        <v>184</v>
-      </c>
-      <c r="F15" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
@@ -2769,16 +3147,16 @@
         <v>95</v>
       </c>
       <c r="C17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E17" t="s">
+        <v>182</v>
+      </c>
+      <c r="F17" t="s">
         <v>176</v>
-      </c>
-      <c r="E17" t="s">
-        <v>183</v>
-      </c>
-      <c r="F17" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
@@ -2786,16 +3164,16 @@
         <v>91</v>
       </c>
       <c r="C18" t="s">
+        <v>176</v>
+      </c>
+      <c r="D18" t="s">
+        <v>175</v>
+      </c>
+      <c r="E18" t="s">
+        <v>182</v>
+      </c>
+      <c r="F18" t="s">
         <v>177</v>
-      </c>
-      <c r="D18" t="s">
-        <v>176</v>
-      </c>
-      <c r="E18" t="s">
-        <v>183</v>
-      </c>
-      <c r="F18" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
@@ -2803,13 +3181,13 @@
         <v>86</v>
       </c>
       <c r="C19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
@@ -2849,7 +3227,7 @@
         <v>47</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="N25" t="s">
         <v>112</v>
@@ -3051,7 +3429,7 @@
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B36" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.25">
@@ -3078,32 +3456,32 @@
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B40" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B41" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B42" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B43" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
L5Min - Bypassed 404 url not found
</commit_message>
<xml_diff>
--- a/BballMVC/_Documentation/BballMVC_Doc.xlsx
+++ b/BballMVC/_Documentation/BballMVC_Doc.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\wwwroot\Test\mrroot123\mrroot123\BballMVCproject\BballMVC\_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A810E7E1-0795-4063-BE5E-21FA0E8CDD48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559AC4E2-CF75-4C49-8DB3-D9936CF972DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30855" yWindow="255" windowWidth="26265" windowHeight="14280" activeTab="1" xr2:uid="{03DA9A79-FE21-4B9D-9E56-4EA80CA75797}"/>
+    <workbookView xWindow="30645" yWindow="60" windowWidth="25200" windowHeight="13365" activeTab="2" xr2:uid="{03DA9A79-FE21-4B9D-9E56-4EA80CA75797}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="3" r:id="rId1"/>
     <sheet name="Tables" sheetId="1" r:id="rId2"/>
-    <sheet name="References" sheetId="2" r:id="rId3"/>
-    <sheet name="DLLs" sheetId="7" r:id="rId4"/>
-    <sheet name="UI Adj Page" sheetId="4" r:id="rId5"/>
-    <sheet name="Adj Point Pct" sheetId="5" r:id="rId6"/>
-    <sheet name="Pt Value Analysis" sheetId="8" r:id="rId7"/>
+    <sheet name="SeasonInfo" sheetId="9" r:id="rId3"/>
+    <sheet name="References" sheetId="2" r:id="rId4"/>
+    <sheet name="DLLs" sheetId="7" r:id="rId5"/>
+    <sheet name="UI Adj Page" sheetId="4" r:id="rId6"/>
+    <sheet name="Adj Point Pct" sheetId="5" r:id="rId7"/>
+    <sheet name="Pt Value Analysis" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tables!$A$1:$P$25</definedName>
@@ -83,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="244">
   <si>
     <t>Table</t>
   </si>
@@ -1059,12 +1060,63 @@
   <si>
     <t>sync</t>
   </si>
+  <si>
+    <t>LeagueInfoID</t>
+  </si>
+  <si>
+    <t>LeagueName</t>
+  </si>
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>EndDate</t>
+  </si>
+  <si>
+    <t>Season</t>
+  </si>
+  <si>
+    <t>SubSeason</t>
+  </si>
+  <si>
+    <t>Bypass</t>
+  </si>
+  <si>
+    <t>IncludePre</t>
+  </si>
+  <si>
+    <t>IncludePost</t>
+  </si>
+  <si>
+    <t>BoxscoreSource</t>
+  </si>
+  <si>
+    <t>NBA</t>
+  </si>
+  <si>
+    <t>0-Pre</t>
+  </si>
+  <si>
+    <t>BB-Ref</t>
+  </si>
+  <si>
+    <t>1-Reg</t>
+  </si>
+  <si>
+    <t>1-AllStarBreak</t>
+  </si>
+  <si>
+    <t>2-Post</t>
+  </si>
+  <si>
+    <t>3-End</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1125,6 +1177,13 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1312,7 +1371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1388,6 +1447,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2040,7 +2101,7 @@
   <sheetPr codeName="Sheet2" filterMode="1"/>
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
@@ -2826,6 +2887,262 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{128C6717-6AF0-4DAB-98D5-EEEAD19CDDB8}">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="A2:J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="47">
+        <v>67</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>237</v>
+      </c>
+      <c r="C2" s="48">
+        <v>44178</v>
+      </c>
+      <c r="D2" s="48">
+        <v>44186</v>
+      </c>
+      <c r="E2" s="47">
+        <v>2021</v>
+      </c>
+      <c r="F2" s="47" t="s">
+        <v>238</v>
+      </c>
+      <c r="G2" s="47">
+        <v>0</v>
+      </c>
+      <c r="H2" s="47">
+        <v>1</v>
+      </c>
+      <c r="I2" s="47">
+        <v>0</v>
+      </c>
+      <c r="J2" s="47" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C3" s="35">
+        <f>D2+1</f>
+        <v>44187</v>
+      </c>
+      <c r="D3" s="35">
+        <v>44238</v>
+      </c>
+      <c r="E3">
+        <f>E2</f>
+        <v>2021</v>
+      </c>
+      <c r="F3" t="s">
+        <v>240</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>69</v>
+      </c>
+      <c r="B4" t="s">
+        <v>237</v>
+      </c>
+      <c r="C4" s="35">
+        <f t="shared" ref="C4:C7" si="0">D3+1</f>
+        <v>44239</v>
+      </c>
+      <c r="D4" s="35">
+        <v>44248</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E7" si="1">E3</f>
+        <v>2021</v>
+      </c>
+      <c r="F4" t="s">
+        <v>241</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
+        <v>237</v>
+      </c>
+      <c r="C5" s="35">
+        <f t="shared" si="0"/>
+        <v>44249</v>
+      </c>
+      <c r="D5" s="35">
+        <v>44332</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>2021</v>
+      </c>
+      <c r="F5" t="s">
+        <v>240</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>135</v>
+      </c>
+      <c r="B6" t="s">
+        <v>237</v>
+      </c>
+      <c r="C6" s="35">
+        <f t="shared" si="0"/>
+        <v>44333</v>
+      </c>
+      <c r="D6" s="35">
+        <v>44383</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>2021</v>
+      </c>
+      <c r="F6" t="s">
+        <v>242</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>138</v>
+      </c>
+      <c r="B7" t="s">
+        <v>237</v>
+      </c>
+      <c r="C7" s="35">
+        <f t="shared" si="0"/>
+        <v>44384</v>
+      </c>
+      <c r="D7" s="35">
+        <v>44484</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>2021</v>
+      </c>
+      <c r="F7" t="s">
+        <v>243</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>239</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE5D99A2-B987-4E19-A171-ABA2F3A75912}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Q45"/>
@@ -3553,7 +3870,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F62BD8A-AB80-4EAF-ADD1-A729FC57348B}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="D2"/>
@@ -3579,7 +3896,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF307F37-89F6-4478-B427-6D1C32C2CB55}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B7:B32"/>
@@ -3673,7 +3990,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{133B7AB1-EBB5-464D-9336-80F19EC6C35C}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:D10"/>
@@ -3774,7 +4091,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C17B75FB-3788-4C0A-A5BD-D95698756B72}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:F11"/>

</xml_diff>